<commit_message>
first speed measurement added
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\multiprocessors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9215F909-77B5-43E2-9F49-4CD7C3E7D873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642211D4-271B-4CA5-BD80-9A9530621810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9045" yWindow="2070" windowWidth="25725" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18420" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,9 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2">
+        <v>2650.7782999999999</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -503,7 +505,9 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2">
+        <v>1894.2938999999999</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -518,7 +522,9 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2">
+        <v>16164.9395</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -547,7 +553,9 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <v>120.9529</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>

</xml_diff>

<commit_message>
changes in openmp added
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\multiprocessors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A559DCDC-3F0C-40D7-9F37-B8022B10CFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9484FAE-62A7-45B7-923C-5EB3CAB41FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18555" yWindow="990" windowWidth="19575" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18645" yWindow="1125" windowWidth="19575" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:G18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +567,9 @@
       <c r="G5" s="2">
         <v>1218.4000000000001</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>1784.4763</v>
+      </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -606,7 +608,9 @@
       <c r="G7" s="2">
         <v>456.3</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>63.197000000000003</v>
+      </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -631,7 +635,9 @@
       <c r="G8" s="2">
         <v>55.1</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>215.2483</v>
+      </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -686,6 +692,9 @@
       <c r="G11">
         <v>352.2</v>
       </c>
+      <c r="H11" s="2">
+        <v>290.61660000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -709,6 +718,9 @@
       <c r="G12">
         <v>122.8</v>
       </c>
+      <c r="H12" s="2">
+        <v>990.41700000000003</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -740,6 +752,9 @@
       </c>
       <c r="G14">
         <v>1118.5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1771.2599</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -833,9 +848,13 @@
         <f>E5/F5</f>
         <v>5.7255940668987435</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="4">
         <f>E5/G5</f>
         <v>6.209619172685489</v>
+      </c>
+      <c r="H19" s="3">
+        <f>C5/H5</f>
+        <v>9.0586462257862426</v>
       </c>
       <c r="I19" s="2"/>
     </row>
@@ -857,7 +876,7 @@
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="3">
         <f>E7/F7</f>
         <v>3.0297029702970297</v>
       </c>
@@ -865,7 +884,10 @@
         <f>E7/G7</f>
         <v>0.10059171597633136</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <f>C7/H7</f>
+        <v>1.9139025586657594</v>
+      </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -879,11 +901,14 @@
         <f>E8/F8</f>
         <v>1.9748322147651007</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="4">
         <f>E8/G8</f>
         <v>2.1361161524500907</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="3">
+        <f>C8/H8</f>
+        <v>4.8373250799193306</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -921,9 +946,13 @@
         <f>E11/F11</f>
         <v>1.782814971006853</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="4">
         <f>E11/G11</f>
         <v>1.9204997160704145</v>
+      </c>
+      <c r="H25" s="3">
+        <f>C11/H11</f>
+        <v>5.3753264610486804</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -933,7 +962,7 @@
       <c r="B26" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="4">
         <f>E12/F12</f>
         <v>5.4332514332514332</v>
       </c>
@@ -941,6 +970,10 @@
         <f>E12/G12</f>
         <v>5.4022801302931596</v>
       </c>
+      <c r="H26" s="3">
+        <f>C12/H12</f>
+        <v>6.0236475141278873</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -965,6 +998,10 @@
       <c r="G28" s="2">
         <f>E14/G14</f>
         <v>2.0817165847116677</v>
+      </c>
+      <c r="H28" s="2">
+        <f>C14/H14</f>
+        <v>1.4332865549544704</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>